<commit_message>
robo 06 completo com sucesso
robo 06 webscraping rodando com sucesso
</commit_message>
<xml_diff>
--- a/Dados_empresa.xlsx
+++ b/Dados_empresa.xlsx
@@ -641,6 +641,1043 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Arteplacas Industria de Placas e Artefatos de Metais LTDA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07/01/1985</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Empresa de Pequeno Porte</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Juliana Matheussi Matias</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>29/01/2020</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Thales Juan Volles</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17/01/2019</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Amanda Machado de Campos Tabach</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>21/09/2020</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Valmir Ferreira da Silva</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>07/11/2022</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Arildo Revelino Catafesta</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>23/10/2014</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Michel Gomes Carvalho Cunha</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>03/01/2018</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Invicttus LTDA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Challenge &amp; Leadership Consultoria e Treinamento LTDA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>03/12/2019</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Franciele Schmitz Ronsani</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10/03/2020</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Fernando Andrade dos Santos</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12/03/2021</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Jair Edson Vieira</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>19/04/2013</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Arteplacas Industria de Placas e Artefatos de Metais LTDA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>07/01/1985</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Empresa de Pequeno Porte</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Sabrina Borges Zabala</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>24/02/2022</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Carine Eliza da Silva Oliveira</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17/08/2022</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Amanda Machado de Campos Tabach</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>21/09/2020</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Valmir Ferreira da Silva</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>07/11/2022</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Invicttus LTDA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Franciele Schmitz Ronsani</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>10/03/2020</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Fernando Andrade dos Santos</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12/03/2021</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sabrina Borges Zabala</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>24/02/2022</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Carine Eliza da Silva Oliveira</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>17/08/2022</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Bruno Stolf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>11/02/2020</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Dionei Seibt</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Daiane de Oliveira</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16/12/2020</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Jose Luiz Pimentel</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>17/08/2022</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Metas Treinamento em Desenvolvimento Profissional e Gerencial LTDA</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Fratello Textil LTDA</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Jeferson Schiblski</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>30/12/2020</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Barbara Cristina Trindade Mazzoleni Chagas da Silva</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>27/05/2020</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Jean Carlo Martins</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>07/11/2022</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Plr Servicos Administrativos LTDA</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>03/12/2020</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Ivete Silva dos Santos Cancissu</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Carla Caroline dos Santos Maschio</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07/10/2022</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Casa da Diana LTDA</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Emerson Rodrigo da Silva Rocinholli</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Toni Edemir Ribeiro Constante Junior</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>09/11/2022</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Andre de Lima</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>21/10/2022</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Valmir Ferreira da Silva</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>07/11/2022</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Fernando Andrade dos Santos</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>12/03/2021</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Sabrina Borges Zabala</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>24/02/2022</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Carine Eliza da Silva Oliveira</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>17/08/2022</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Dionei Seibt</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Daiane de Oliveira</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>16/12/2020</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Jose Luiz Pimentel</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17/08/2022</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Jeferson Schiblski</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>30/12/2020</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Jean Carlo Martins</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>07/11/2022</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Plr Servicos Administrativos LTDA</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>03/12/2020</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Ivete Silva dos Santos Cancissu</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Carla Caroline dos Santos Maschio</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>07/10/2022</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Casa da Diana LTDA</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Emerson Rodrigo da Silva Rocinholli</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>10/09/2021</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Toni Edemir Ribeiro Constante Junior</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>09/11/2022</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Andre de Lima</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>21/10/2022</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Jessica Aparecida de Morais</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>25/11/2020</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Oral Unic Odontologia Itapira LTDA</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>21/10/2022</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Sem Enquadramento</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Cleber Scaburri</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>07/10/2022</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Kaue Eduardo Ribeiro Felters</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>25/11/2020</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Raquel Edith Loos</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>09/02/2021</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Micro Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Lucas Batista dos Santos Silva</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>17/03/2021</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Sergio Wanzynack</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>17/03/2021</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Microempreendendor Individual (MEI)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>